<commit_message>
Minor changes to CDCM statistics.
</commit_message>
<xml_diff>
--- a/Summaries/CDCM stats table 4201.xlsx
+++ b/Summaries/CDCM stats table 4201.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="16320" tabRatio="500"/>
@@ -10,7 +10,7 @@
     <sheet name="4201" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'4201'!$A$3:$M$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'4201'!$A$3:$M$30</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>Capacity (kVA)</t>
   </si>
@@ -45,15 +45,9 @@
     <t>Tariff selection</t>
   </si>
   <si>
-    <t>^(?:LV|LV Sub|HV|LDNO .*) HH Metered$</t>
-  </si>
-  <si>
     <t>Load factor (kW/kVA)</t>
   </si>
   <si>
-    <t>^(?:|LDNO .*)HV HH Metered$</t>
-  </si>
-  <si>
     <t>Electric home</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>Domestic electric heat</t>
   </si>
   <si>
-    <t>Generator</t>
-  </si>
-  <si>
     <t>Medium housing electric</t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>XL housing standard</t>
   </si>
   <si>
-    <t>^HV.*Gener</t>
-  </si>
-  <si>
     <t>(?:^|: )(?:LV Network Domestic|Domestic [UT])</t>
   </si>
   <si>
@@ -217,19 +205,41 @@
   </si>
   <si>
     <t>Average rate 2 kWh/year</t>
+  </si>
+  <si>
+    <t>All-the-way generation</t>
+  </si>
+  <si>
+    <t>^(?:|LDNO .*: )HV HH Metered$</t>
+  </si>
+  <si>
+    <t>^(?:LV|LV Sub|HV|LDNO .*:) HH Metered$</t>
+  </si>
+  <si>
+    <t>All-the-way demand</t>
+  </si>
+  <si>
+    <t>Other demand (1)</t>
+  </si>
+  <si>
+    <t>Other demand (2)</t>
+  </si>
+  <si>
+    <t>Other generation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="\ _(???,???,??0_);[Red]\ \(???,???,??0\);;@"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="??0.0%"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -356,7 +366,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="477">
+  <cellStyleXfs count="493">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -490,6 +500,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -858,15 +884,8 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="132" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -895,8 +914,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="477">
+  <cellStyles count="493">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1135,6 +1161,14 @@
     <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1372,6 +1406,14 @@
     <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="132" builtinId="5"/>
   </cellStyles>
@@ -1702,7 +1744,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1719,7 +1761,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="19">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1732,7 +1774,7 @@
     </row>
     <row r="3" spans="1:13" ht="28">
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -1756,1096 +1798,1096 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="8">
+        <v>34</v>
+      </c>
+      <c r="B4" s="7">
         <v>110</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>19</v>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="5">
-        <f>D$34</f>
+        <f>D$37</f>
         <v>66</v>
       </c>
       <c r="E4" s="5">
-        <f>E$34</f>
+        <f>E$37</f>
         <v>0</v>
       </c>
       <c r="F4" s="6">
-        <f>F$34*$I4</f>
+        <f>F$37*$I4</f>
         <v>16.099999999999998</v>
       </c>
       <c r="G4" s="6">
-        <f>G$34*$I4</f>
+        <f>G$37*$I4</f>
         <v>0</v>
       </c>
       <c r="H4" s="6">
-        <f>H$34*$I4</f>
+        <f>H$37*$I4</f>
         <v>4.7352941176470598</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="16">
         <v>23</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="17">
         <f>(D4*F4+E4*G4+(168-D4-E4)*H4)*365.25/7</f>
         <v>80647.199999999997</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="17">
         <f>E4*G4*365.25/7</f>
         <v>0</v>
       </c>
-      <c r="L4" s="10">
-        <f t="shared" ref="L4:L29" si="0">J4/365/24/I4</f>
-        <v>0.40027397260273967</v>
-      </c>
-      <c r="M4" s="11">
-        <f t="shared" ref="M4:M29" si="1">MAX(F4,H4)/J4*365*24</f>
-        <v>1.7488021902806294</v>
+      <c r="L4" s="8">
+        <f>J4/365.25/24/I4</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M4" s="9">
+        <f>MAX(F4,H4)/J4*365.25*24</f>
+        <v>1.7499999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="8">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7">
         <v>120</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>19</v>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="5">
-        <f>D$36</f>
+        <f>D$39</f>
         <v>0</v>
       </c>
       <c r="E5" s="5">
-        <f>E$36</f>
+        <f>E$39</f>
         <v>0</v>
       </c>
       <c r="F5" s="6">
-        <f>F$36*$I5</f>
+        <f>F$39*$I5</f>
         <v>0</v>
       </c>
       <c r="G5" s="6">
-        <f>G$36*$I5</f>
+        <f>G$39*$I5</f>
         <v>0</v>
       </c>
       <c r="H5" s="6">
-        <f>H$36*$I5</f>
+        <f>H$39*$I5</f>
         <v>20.7</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="16">
         <v>23</v>
       </c>
-      <c r="J5" s="9">
-        <f t="shared" ref="J5:J29" si="2">(D5*F5+E5*G5+(168-D5-E5)*H5)*365.25/7</f>
+      <c r="J5" s="17">
+        <f t="shared" ref="J5:J30" si="0">(D5*F5+E5*G5+(168-D5-E5)*H5)*365.25/7</f>
         <v>181456.19999999998</v>
       </c>
-      <c r="K5" s="9">
-        <f t="shared" ref="K5:K29" si="3">E5*G5*365.25/7</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="10">
-        <f t="shared" si="0"/>
-        <v>0.90061643835616434</v>
-      </c>
-      <c r="M5" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+      <c r="K5" s="17">
+        <f t="shared" ref="K5:K30" si="1">E5*G5*365.25/7</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" ref="L5:L31" si="2">J5/365.25/24/I5</f>
+        <v>0.9</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" ref="M5:M31" si="3">MAX(F5,H5)/J5*365.25*24</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="8">
+        <v>32</v>
+      </c>
+      <c r="B6" s="7">
         <v>130</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>19</v>
+      <c r="C6" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D6" s="5">
-        <f>D$35</f>
+        <f>D$38</f>
         <v>0</v>
       </c>
       <c r="E6" s="5">
-        <f>E$35</f>
+        <f>E$38</f>
         <v>74.666666666666671</v>
       </c>
       <c r="F6" s="6">
-        <f>F$35*$I6</f>
+        <f>F$38*$I6</f>
         <v>0</v>
       </c>
       <c r="G6" s="6">
-        <f>G$35*$I6</f>
+        <f>G$38*$I6</f>
         <v>20.7</v>
       </c>
       <c r="H6" s="6">
-        <f>H$35*$I6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="7">
+        <f>H$38*$I6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="16">
         <v>23</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="17">
+        <f t="shared" si="0"/>
+        <v>80647.199999999997</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" si="1"/>
+        <v>80647.199999999997</v>
+      </c>
+      <c r="L6" s="8">
         <f t="shared" si="2"/>
-        <v>80647.199999999997</v>
-      </c>
-      <c r="K6" s="9">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M6" s="9">
         <f t="shared" si="3"/>
-        <v>80647.199999999997</v>
-      </c>
-      <c r="L6" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273967</v>
-      </c>
-      <c r="M6" s="11">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="8">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7">
         <v>145</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>19</v>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="5">
-        <f>D$37</f>
+        <f>D$40</f>
         <v>0</v>
       </c>
       <c r="E7" s="5">
-        <f>E$37</f>
+        <f>E$40</f>
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <f>F$37*$I7</f>
+        <f>F$40*$I7</f>
         <v>0</v>
       </c>
       <c r="G7" s="6">
-        <f>G$37*$I7</f>
+        <f>G$40*$I7</f>
         <v>0</v>
       </c>
       <c r="H7" s="6">
-        <f>H$37*$I7</f>
+        <f>H$40*$I7</f>
         <v>9.2000000000000011</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="16">
         <v>23</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="17">
+        <f t="shared" si="0"/>
+        <v>80647.199999999997</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
         <f t="shared" si="2"/>
-        <v>80647.199999999997</v>
-      </c>
-      <c r="K7" s="9">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M7" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273967</v>
-      </c>
-      <c r="M7" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="8">
+        <v>38</v>
+      </c>
+      <c r="B8" s="7">
         <f>100+B4</f>
         <v>210</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>18</v>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D8" s="5">
-        <f>D$34</f>
+        <f>D$37</f>
         <v>66</v>
       </c>
       <c r="E8" s="5">
-        <f>E$34</f>
+        <f>E$37</f>
         <v>0</v>
       </c>
       <c r="F8" s="6">
-        <f>F$34*$I8</f>
+        <f>F$37*$I8</f>
         <v>48.3</v>
       </c>
       <c r="G8" s="6">
-        <f>G$34*$I8</f>
+        <f>G$37*$I8</f>
         <v>0</v>
       </c>
       <c r="H8" s="6">
-        <f>H$34*$I8</f>
+        <f>H$37*$I8</f>
         <v>14.205882352941179</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="16">
         <v>69</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="17">
+        <f t="shared" si="0"/>
+        <v>241941.6</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
         <f t="shared" si="2"/>
-        <v>241941.6</v>
-      </c>
-      <c r="K8" s="9">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M8" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273972</v>
-      </c>
-      <c r="M8" s="11">
-        <f t="shared" si="1"/>
-        <v>1.7488021902806294</v>
+        <v>1.7499999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="8">
+        <v>39</v>
+      </c>
+      <c r="B9" s="7">
         <f>100+B5</f>
         <v>220</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>18</v>
+      <c r="C9" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D9" s="5">
-        <f>D$36</f>
+        <f>D$39</f>
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <f>E$36</f>
+        <f>E$39</f>
         <v>0</v>
       </c>
       <c r="F9" s="6">
-        <f>F$36*$I9</f>
+        <f>F$39*$I9</f>
         <v>0</v>
       </c>
       <c r="G9" s="6">
-        <f>G$36*$I9</f>
+        <f>G$39*$I9</f>
         <v>0</v>
       </c>
       <c r="H9" s="6">
-        <f>H$36*$I9</f>
+        <f>H$39*$I9</f>
         <v>62.1</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="16">
         <v>69</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="17">
+        <f t="shared" si="0"/>
+        <v>544368.6</v>
+      </c>
+      <c r="K9" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="8">
         <f t="shared" si="2"/>
-        <v>544368.6</v>
-      </c>
-      <c r="K9" s="9">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="M9" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="10">
-        <f t="shared" si="0"/>
-        <v>0.90061643835616434</v>
-      </c>
-      <c r="M9" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="8">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7">
         <f>100+B6</f>
         <v>230</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>18</v>
+      <c r="C10" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="5">
-        <f>D$35</f>
+        <f>D$38</f>
         <v>0</v>
       </c>
       <c r="E10" s="5">
-        <f>E$35</f>
+        <f>E$38</f>
         <v>74.666666666666671</v>
       </c>
       <c r="F10" s="6">
-        <f>F$35*$I10</f>
+        <f>F$38*$I10</f>
         <v>0</v>
       </c>
       <c r="G10" s="6">
-        <f>G$35*$I10</f>
+        <f>G$38*$I10</f>
         <v>62.1</v>
       </c>
       <c r="H10" s="6">
-        <f>H$35*$I10</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="7">
+        <f>H$38*$I10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="16">
         <v>69</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="17">
+        <f t="shared" si="0"/>
+        <v>241941.6</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="1"/>
+        <v>241941.6</v>
+      </c>
+      <c r="L10" s="8">
         <f t="shared" si="2"/>
-        <v>241941.6</v>
-      </c>
-      <c r="K10" s="9">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M10" s="9">
         <f t="shared" si="3"/>
-        <v>241941.6</v>
-      </c>
-      <c r="L10" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273972</v>
-      </c>
-      <c r="M10" s="11">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="8">
+        <v>37</v>
+      </c>
+      <c r="B11" s="7">
         <f>100+B7</f>
         <v>245</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>18</v>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="5">
-        <f>D$37</f>
+        <f>D$40</f>
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <f>E$37</f>
+        <f>E$40</f>
         <v>0</v>
       </c>
       <c r="F11" s="6">
-        <f>F$37*$I11</f>
+        <f>F$40*$I11</f>
         <v>0</v>
       </c>
       <c r="G11" s="6">
-        <f>G$37*$I11</f>
+        <f>G$40*$I11</f>
         <v>0</v>
       </c>
       <c r="H11" s="6">
-        <f>H$37*$I11</f>
+        <f>H$40*$I11</f>
         <v>27.6</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="16">
         <v>69</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="17">
+        <f t="shared" si="0"/>
+        <v>241941.6</v>
+      </c>
+      <c r="K11" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
         <f t="shared" si="2"/>
-        <v>241941.6</v>
-      </c>
-      <c r="K11" s="9">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M11" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273972</v>
-      </c>
-      <c r="M11" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="8">
+        <v>51</v>
+      </c>
+      <c r="B12" s="7">
         <v>255</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>18</v>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D12" s="5">
-        <f>D$33</f>
+        <f>D$36</f>
         <v>35</v>
       </c>
       <c r="E12" s="5">
-        <f>E$33</f>
+        <f>E$36</f>
         <v>49</v>
       </c>
       <c r="F12" s="6">
-        <f>10*F$33</f>
+        <f>10*F$36</f>
         <v>11</v>
       </c>
       <c r="G12" s="6">
-        <f>10*G$33</f>
+        <f>10*G$36</f>
         <v>16</v>
       </c>
       <c r="H12" s="6">
-        <f>10*H$33</f>
+        <f>10*H$36</f>
         <v>4.3481735159817365</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="16">
         <v>69</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="17">
+        <f t="shared" si="0"/>
+        <v>80054.794520547948</v>
+      </c>
+      <c r="K12" s="17">
+        <f t="shared" si="1"/>
+        <v>40908</v>
+      </c>
+      <c r="L12" s="8">
         <f t="shared" si="2"/>
-        <v>80054.794520547948</v>
-      </c>
-      <c r="K12" s="9">
+        <v>0.13235391436701741</v>
+      </c>
+      <c r="M12" s="9">
         <f t="shared" si="3"/>
-        <v>40908</v>
-      </c>
-      <c r="L12" s="10">
-        <f t="shared" si="0"/>
-        <v>0.13244456773302221</v>
-      </c>
-      <c r="M12" s="11">
-        <f t="shared" si="1"/>
-        <v>1.2036755646817248</v>
+        <v>1.2044999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="8">
+        <v>52</v>
+      </c>
+      <c r="B13" s="7">
         <v>265</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>18</v>
+      <c r="C13" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D13" s="5">
-        <f>D$32</f>
+        <f>D$35</f>
         <v>35</v>
       </c>
       <c r="E13" s="5">
-        <f>E$32</f>
+        <f>E$35</f>
         <v>49</v>
       </c>
       <c r="F13" s="6">
-        <f>25*F$32</f>
+        <f>25*F$35</f>
         <v>20</v>
       </c>
       <c r="G13" s="6">
-        <f>25*G$32</f>
+        <f>25*G$35</f>
         <v>6.25</v>
       </c>
       <c r="H13" s="6">
-        <f>25*H$32</f>
+        <f>25*H$35</f>
         <v>9.7103310502283122</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="16">
         <v>69</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="17">
+        <f t="shared" si="0"/>
+        <v>95065.068493150713</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="1"/>
+        <v>15979.6875</v>
+      </c>
+      <c r="L13" s="8">
         <f t="shared" si="2"/>
-        <v>95065.068493150713</v>
-      </c>
-      <c r="K13" s="9">
+        <v>0.15717027331083319</v>
+      </c>
+      <c r="M13" s="9">
         <f t="shared" si="3"/>
-        <v>15979.6875</v>
-      </c>
-      <c r="L13" s="10">
-        <f t="shared" si="0"/>
-        <v>0.15727792418296391</v>
-      </c>
-      <c r="M13" s="11">
-        <f t="shared" si="1"/>
-        <v>1.8429482330055111</v>
+        <v>1.8442105263157886</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="8">
+        <v>42</v>
+      </c>
+      <c r="B14" s="7">
         <f t="shared" ref="B14:B25" si="4">B8+100</f>
         <v>310</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>7</v>
+      <c r="C14" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D14" s="5">
-        <f>D$34</f>
+        <f>D$37</f>
         <v>66</v>
       </c>
       <c r="E14" s="5">
-        <f>E$34</f>
+        <f>E$37</f>
         <v>0</v>
       </c>
       <c r="F14" s="6">
-        <f>F$34*$I14</f>
+        <f>F$37*$I14</f>
         <v>350</v>
       </c>
       <c r="G14" s="6">
-        <f>G$34*$I14</f>
+        <f>G$37*$I14</f>
         <v>0</v>
       </c>
       <c r="H14" s="6">
-        <f>H$34*$I14</f>
+        <f>H$37*$I14</f>
         <v>102.94117647058826</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="16">
         <v>500</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="17">
+        <f t="shared" si="0"/>
+        <v>1753200</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="8">
         <f t="shared" si="2"/>
-        <v>1753200</v>
-      </c>
-      <c r="K14" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="M14" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273978</v>
-      </c>
-      <c r="M14" s="11">
-        <f t="shared" si="1"/>
-        <v>1.7488021902806299</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="8">
+        <v>43</v>
+      </c>
+      <c r="B15" s="7">
         <f t="shared" si="4"/>
         <v>320</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>7</v>
+      <c r="C15" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D15" s="5">
-        <f>D$36</f>
+        <f>D$39</f>
         <v>0</v>
       </c>
       <c r="E15" s="5">
-        <f>E$36</f>
+        <f>E$39</f>
         <v>0</v>
       </c>
       <c r="F15" s="6">
-        <f>F$36*$I15</f>
+        <f>F$39*$I15</f>
         <v>0</v>
       </c>
       <c r="G15" s="6">
-        <f>G$36*$I15</f>
+        <f>G$39*$I15</f>
         <v>0</v>
       </c>
       <c r="H15" s="6">
-        <f>H$36*$I15</f>
+        <f>H$39*$I15</f>
         <v>450</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="16">
         <v>500</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="17">
+        <f t="shared" si="0"/>
+        <v>3944700</v>
+      </c>
+      <c r="K15" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="8">
         <f t="shared" si="2"/>
-        <v>3944700</v>
-      </c>
-      <c r="K15" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="M15" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="10">
-        <f t="shared" si="0"/>
-        <v>0.90061643835616434</v>
-      </c>
-      <c r="M15" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="8">
+      <c r="A16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="7">
         <f t="shared" si="4"/>
         <v>330</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>7</v>
+      <c r="C16" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D16" s="5">
-        <f>D$35</f>
+        <f>D$38</f>
         <v>0</v>
       </c>
       <c r="E16" s="5">
-        <f>E$35</f>
+        <f>E$38</f>
         <v>74.666666666666671</v>
       </c>
       <c r="F16" s="6">
-        <f>F$35*$I16</f>
+        <f>F$38*$I16</f>
         <v>0</v>
       </c>
       <c r="G16" s="6">
-        <f>G$35*$I16</f>
+        <f>G$38*$I16</f>
         <v>450</v>
       </c>
       <c r="H16" s="6">
-        <f>H$35*$I16</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="7">
+        <f>H$38*$I16</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="16">
         <v>500</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="17">
+        <f t="shared" si="0"/>
+        <v>1753200</v>
+      </c>
+      <c r="K16" s="17">
+        <f t="shared" si="1"/>
+        <v>1753200</v>
+      </c>
+      <c r="L16" s="8">
         <f t="shared" si="2"/>
-        <v>1753200</v>
-      </c>
-      <c r="K16" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="M16" s="9">
         <f t="shared" si="3"/>
-        <v>1753200</v>
-      </c>
-      <c r="L16" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273978</v>
-      </c>
-      <c r="M16" s="11">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="8">
+        <v>41</v>
+      </c>
+      <c r="B17" s="7">
         <f t="shared" si="4"/>
         <v>345</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>7</v>
+      <c r="C17" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D17" s="5">
-        <f>D$37</f>
+        <f>D$40</f>
         <v>0</v>
       </c>
       <c r="E17" s="5">
-        <f>E$37</f>
+        <f>E$40</f>
         <v>0</v>
       </c>
       <c r="F17" s="6">
-        <f>F$37*$I17</f>
+        <f>F$40*$I17</f>
         <v>0</v>
       </c>
       <c r="G17" s="6">
-        <f>G$37*$I17</f>
+        <f>G$40*$I17</f>
         <v>0</v>
       </c>
       <c r="H17" s="6">
-        <f>H$37*$I17</f>
+        <f>H$40*$I17</f>
         <v>200</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="16">
         <v>500</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="17">
+        <f t="shared" si="0"/>
+        <v>1753200</v>
+      </c>
+      <c r="K17" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="8">
         <f t="shared" si="2"/>
-        <v>1753200</v>
-      </c>
-      <c r="K17" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="M17" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273978</v>
-      </c>
-      <c r="M17" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="8">
+      <c r="A18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="7">
         <f t="shared" si="4"/>
         <v>355</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>7</v>
+      <c r="C18" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D18" s="5">
-        <f>D$33</f>
+        <f>D$36</f>
         <v>35</v>
       </c>
       <c r="E18" s="5">
-        <f>E$33</f>
+        <f>E$36</f>
         <v>49</v>
       </c>
       <c r="F18" s="6">
-        <f>100*F$33</f>
+        <f>100*F$36</f>
         <v>110.00000000000001</v>
       </c>
       <c r="G18" s="6">
-        <f>100*G$33</f>
+        <f>100*G$36</f>
         <v>160</v>
       </c>
       <c r="H18" s="6">
-        <f>100*H$33</f>
+        <f>100*H$36</f>
         <v>43.481735159817362</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="16">
         <v>500</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="17">
+        <f t="shared" si="0"/>
+        <v>800547.94520547951</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="1"/>
+        <v>409080</v>
+      </c>
+      <c r="L18" s="8">
         <f t="shared" si="2"/>
-        <v>800547.94520547951</v>
-      </c>
-      <c r="K18" s="9">
+        <v>0.18264840182648401</v>
+      </c>
+      <c r="M18" s="9">
         <f t="shared" si="3"/>
-        <v>409080</v>
-      </c>
-      <c r="L18" s="10">
-        <f t="shared" si="0"/>
-        <v>0.18277350347157065</v>
-      </c>
-      <c r="M18" s="11">
-        <f t="shared" si="1"/>
-        <v>1.203675564681725</v>
+        <v>1.2045000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="8">
+        <v>54</v>
+      </c>
+      <c r="B19" s="7">
         <f t="shared" si="4"/>
         <v>365</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>7</v>
+      <c r="C19" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D19" s="5">
-        <f>D$32</f>
+        <f>D$35</f>
         <v>35</v>
       </c>
       <c r="E19" s="5">
-        <f>E$32</f>
+        <f>E$35</f>
         <v>49</v>
       </c>
       <c r="F19" s="6">
-        <f>250*F$32</f>
+        <f>250*F$35</f>
         <v>200</v>
       </c>
       <c r="G19" s="6">
-        <f>250*G$32</f>
+        <f>250*G$35</f>
         <v>62.5</v>
       </c>
       <c r="H19" s="6">
-        <f>250*H$32</f>
+        <f>250*H$35</f>
         <v>97.103310502283136</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="16">
         <v>500</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="17">
+        <f t="shared" si="0"/>
+        <v>950650.6849315071</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="1"/>
+        <v>159796.875</v>
+      </c>
+      <c r="L19" s="8">
         <f t="shared" si="2"/>
-        <v>950650.6849315071</v>
-      </c>
-      <c r="K19" s="9">
+        <v>0.21689497716894982</v>
+      </c>
+      <c r="M19" s="9">
         <f t="shared" si="3"/>
-        <v>159796.875</v>
-      </c>
-      <c r="L19" s="10">
-        <f t="shared" si="0"/>
-        <v>0.21704353537249019</v>
-      </c>
-      <c r="M19" s="11">
-        <f t="shared" si="1"/>
-        <v>1.8429482330055116</v>
+        <v>1.8442105263157891</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="8">
+        <v>46</v>
+      </c>
+      <c r="B20" s="7">
         <f t="shared" si="4"/>
         <v>410</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>9</v>
+      <c r="C20" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D20" s="5">
-        <f>D$34</f>
+        <f>D$37</f>
         <v>66</v>
       </c>
       <c r="E20" s="5">
-        <f>E$34</f>
+        <f>E$37</f>
         <v>0</v>
       </c>
       <c r="F20" s="6">
-        <f>F$34*$I20</f>
+        <f>F$37*$I20</f>
         <v>3500</v>
       </c>
       <c r="G20" s="6">
-        <f>G$34*$I20</f>
+        <f>G$37*$I20</f>
         <v>0</v>
       </c>
       <c r="H20" s="6">
-        <f>H$34*$I20</f>
+        <f>H$37*$I20</f>
         <v>1029.4117647058827</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="16">
         <v>5000</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="17">
+        <f t="shared" si="0"/>
+        <v>17532000</v>
+      </c>
+      <c r="K20" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="8">
         <f t="shared" si="2"/>
-        <v>17532000</v>
-      </c>
-      <c r="K20" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="M20" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273972</v>
-      </c>
-      <c r="M20" s="11">
-        <f t="shared" si="1"/>
-        <v>1.7488021902806299</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="8">
+        <v>47</v>
+      </c>
+      <c r="B21" s="7">
         <f t="shared" si="4"/>
         <v>420</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>9</v>
+      <c r="C21" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D21" s="5">
-        <f>D$36</f>
+        <f>D$39</f>
         <v>0</v>
       </c>
       <c r="E21" s="5">
-        <f>E$36</f>
+        <f>E$39</f>
         <v>0</v>
       </c>
       <c r="F21" s="6">
-        <f>F$36*$I21</f>
+        <f>F$39*$I21</f>
         <v>0</v>
       </c>
       <c r="G21" s="6">
-        <f>G$36*$I21</f>
+        <f>G$39*$I21</f>
         <v>0</v>
       </c>
       <c r="H21" s="6">
-        <f>H$36*$I21</f>
+        <f>H$39*$I21</f>
         <v>4500</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="16">
         <v>5000</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="17">
+        <f t="shared" si="0"/>
+        <v>39447000</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
         <f t="shared" si="2"/>
-        <v>39447000</v>
-      </c>
-      <c r="K21" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="M21" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="10">
-        <f t="shared" si="0"/>
-        <v>0.90061643835616434</v>
-      </c>
-      <c r="M21" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="8">
+        <v>44</v>
+      </c>
+      <c r="B22" s="7">
         <f t="shared" si="4"/>
         <v>430</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>9</v>
+      <c r="C22" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D22" s="5">
-        <f>D$35</f>
+        <f>D$38</f>
         <v>0</v>
       </c>
       <c r="E22" s="5">
-        <f>E$35</f>
+        <f>E$38</f>
         <v>74.666666666666671</v>
       </c>
       <c r="F22" s="6">
-        <f>F$35*$I22</f>
+        <f>F$38*$I22</f>
         <v>0</v>
       </c>
       <c r="G22" s="6">
-        <f>G$35*$I22</f>
+        <f>G$38*$I22</f>
         <v>4500</v>
       </c>
       <c r="H22" s="6">
-        <f>H$35*$I22</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="7">
+        <f>H$38*$I22</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="16">
         <v>5000</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="17">
+        <f t="shared" si="0"/>
+        <v>17532000</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="1"/>
+        <v>17532000</v>
+      </c>
+      <c r="L22" s="8">
         <f t="shared" si="2"/>
-        <v>17532000</v>
-      </c>
-      <c r="K22" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="M22" s="9">
         <f t="shared" si="3"/>
-        <v>17532000</v>
-      </c>
-      <c r="L22" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273972</v>
-      </c>
-      <c r="M22" s="11">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="8">
+        <v>45</v>
+      </c>
+      <c r="B23" s="7">
         <f t="shared" si="4"/>
         <v>445</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>9</v>
+      <c r="C23" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D23" s="5">
-        <f>D$37</f>
+        <f>D$40</f>
         <v>0</v>
       </c>
       <c r="E23" s="5">
-        <f>E$37</f>
+        <f>E$40</f>
         <v>0</v>
       </c>
       <c r="F23" s="6">
-        <f>F$37*$I23</f>
+        <f>F$40*$I23</f>
         <v>0</v>
       </c>
       <c r="G23" s="6">
-        <f>G$37*$I23</f>
+        <f>G$40*$I23</f>
         <v>0</v>
       </c>
       <c r="H23" s="6">
-        <f>H$37*$I23</f>
+        <f>H$40*$I23</f>
         <v>2000</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="16">
         <v>5000</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="17">
+        <f t="shared" si="0"/>
+        <v>17532000</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="8">
         <f t="shared" si="2"/>
-        <v>17532000</v>
-      </c>
-      <c r="K23" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="M23" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273972</v>
-      </c>
-      <c r="M23" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="8">
+        <v>55</v>
+      </c>
+      <c r="B24" s="7">
         <f t="shared" si="4"/>
         <v>455</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>9</v>
+      <c r="C24" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D24" s="5">
-        <f>D$33</f>
+        <f>D$36</f>
         <v>35</v>
       </c>
       <c r="E24" s="5">
-        <f>E$33</f>
+        <f>E$36</f>
         <v>49</v>
       </c>
       <c r="F24" s="6">
-        <f>1000*F$33</f>
+        <f>1000*F$36</f>
         <v>1100</v>
       </c>
       <c r="G24" s="6">
-        <f>1000*G$33</f>
+        <f>1000*G$36</f>
         <v>1600</v>
       </c>
       <c r="H24" s="6">
-        <f>1000*H$33</f>
+        <f>1000*H$36</f>
         <v>434.81735159817362</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="16">
         <v>5000</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="17">
+        <f t="shared" si="0"/>
+        <v>8005479.4520547939</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="1"/>
+        <v>4090800</v>
+      </c>
+      <c r="L24" s="8">
         <f t="shared" si="2"/>
-        <v>8005479.4520547939</v>
-      </c>
-      <c r="K24" s="9">
+        <v>0.18264840182648401</v>
+      </c>
+      <c r="M24" s="9">
         <f t="shared" si="3"/>
-        <v>4090800</v>
-      </c>
-      <c r="L24" s="10">
-        <f t="shared" si="0"/>
-        <v>0.18277350347157065</v>
-      </c>
-      <c r="M24" s="11">
-        <f t="shared" si="1"/>
-        <v>1.203675564681725</v>
+        <v>1.2045000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="8">
+      <c r="A25" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="7">
         <f t="shared" si="4"/>
         <v>465</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>9</v>
+      <c r="C25" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" ref="D25:E27" si="5">D$32</f>
+        <f t="shared" ref="D25:E27" si="5">D$35</f>
         <v>35</v>
       </c>
       <c r="E25" s="5">
@@ -2853,46 +2895,46 @@
         <v>49</v>
       </c>
       <c r="F25" s="6">
-        <f>2500*F$32</f>
+        <f>2500*F$35</f>
         <v>2000</v>
       </c>
       <c r="G25" s="6">
-        <f>2500*G$32</f>
+        <f>2500*G$35</f>
         <v>625</v>
       </c>
       <c r="H25" s="6">
-        <f>2500*H$32</f>
+        <f>2500*H$35</f>
         <v>971.03310502283125</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="16">
         <v>5000</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="17">
+        <f t="shared" si="0"/>
+        <v>9506506.8493150678</v>
+      </c>
+      <c r="K25" s="17">
+        <f t="shared" si="1"/>
+        <v>1597968.75</v>
+      </c>
+      <c r="L25" s="8">
         <f t="shared" si="2"/>
-        <v>9506506.8493150678</v>
-      </c>
-      <c r="K25" s="9">
+        <v>0.21689497716894976</v>
+      </c>
+      <c r="M25" s="9">
         <f t="shared" si="3"/>
-        <v>1597968.75</v>
-      </c>
-      <c r="L25" s="10">
-        <f t="shared" si="0"/>
-        <v>0.21704353537249013</v>
-      </c>
-      <c r="M25" s="11">
-        <f t="shared" si="1"/>
-        <v>1.8429482330055118</v>
+        <v>1.8442105263157895</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="8">
+        <v>48</v>
+      </c>
+      <c r="B26" s="7">
         <v>700</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>61</v>
+      <c r="C26" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D26" s="5">
         <f t="shared" si="5"/>
@@ -2903,46 +2945,46 @@
         <v>49</v>
       </c>
       <c r="F26" s="6">
-        <f>F$32/2</f>
+        <f>F$35/2</f>
         <v>0.4</v>
       </c>
       <c r="G26" s="6">
-        <f>G$32/2</f>
+        <f>G$35/2</f>
         <v>0.125</v>
       </c>
       <c r="H26" s="6">
-        <f>H$32/2</f>
+        <f>H$35/2</f>
         <v>0.19420662100456626</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="16">
         <v>6</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="17">
+        <f t="shared" si="0"/>
+        <v>1901.3013698630136</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="1"/>
+        <v>319.59375</v>
+      </c>
+      <c r="L26" s="8">
         <f t="shared" si="2"/>
-        <v>1901.3013698630136</v>
-      </c>
-      <c r="K26" s="9">
+        <v>3.6149162861491627E-2</v>
+      </c>
+      <c r="M26" s="9">
         <f t="shared" si="3"/>
-        <v>319.59375</v>
-      </c>
-      <c r="L26" s="10">
-        <f t="shared" si="0"/>
-        <v>3.6173922562081691E-2</v>
-      </c>
-      <c r="M26" s="11">
-        <f t="shared" si="1"/>
-        <v>1.8429482330055118</v>
+        <v>1.8442105263157895</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="8">
+        <v>49</v>
+      </c>
+      <c r="B27" s="7">
         <v>720</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>61</v>
+      <c r="C27" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="5"/>
@@ -2953,335 +2995,436 @@
         <v>49</v>
       </c>
       <c r="F27" s="6">
-        <f>F$32</f>
+        <f>F$35</f>
         <v>0.8</v>
       </c>
       <c r="G27" s="6">
-        <f>G$32</f>
+        <f>G$35</f>
         <v>0.25</v>
       </c>
       <c r="H27" s="6">
-        <f>H$32</f>
+        <f>H$35</f>
         <v>0.38841324200913252</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="16">
         <v>9</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="17">
+        <f t="shared" si="0"/>
+        <v>3802.6027397260273</v>
+      </c>
+      <c r="K27" s="17">
+        <f t="shared" si="1"/>
+        <v>639.1875</v>
+      </c>
+      <c r="L27" s="8">
         <f t="shared" si="2"/>
-        <v>3802.6027397260273</v>
-      </c>
-      <c r="K27" s="9">
+        <v>4.8198883815322169E-2</v>
+      </c>
+      <c r="M27" s="9">
         <f t="shared" si="3"/>
-        <v>639.1875</v>
-      </c>
-      <c r="L27" s="10">
+        <v>1.8442105263157895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="7">
+        <v>740</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="5">
+        <f>D$36</f>
+        <v>35</v>
+      </c>
+      <c r="E28" s="5">
+        <f>E$36</f>
+        <v>49</v>
+      </c>
+      <c r="F28" s="6">
+        <f>F$36</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G28" s="6">
+        <f>G$36</f>
+        <v>1.6</v>
+      </c>
+      <c r="H28" s="6">
+        <f>H$36</f>
+        <v>0.43481735159817364</v>
+      </c>
+      <c r="I28" s="16">
+        <v>18</v>
+      </c>
+      <c r="J28" s="17">
         <f t="shared" si="0"/>
-        <v>4.8231896749442255E-2</v>
-      </c>
-      <c r="M27" s="11">
+        <v>8005.4794520547957</v>
+      </c>
+      <c r="K28" s="17">
         <f t="shared" si="1"/>
-        <v>1.8429482330055118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="8">
-        <v>740</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="5">
-        <f>D$33</f>
-        <v>35</v>
-      </c>
-      <c r="E28" s="5">
-        <f>E$33</f>
-        <v>49</v>
-      </c>
-      <c r="F28" s="6">
-        <f>F$33</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G28" s="6">
-        <f>G$33</f>
-        <v>1.6</v>
-      </c>
-      <c r="H28" s="6">
-        <f>H$33</f>
-        <v>0.43481735159817364</v>
-      </c>
-      <c r="I28" s="7">
-        <v>18</v>
-      </c>
-      <c r="J28" s="9">
+        <v>4090.8</v>
+      </c>
+      <c r="L28" s="8">
         <f t="shared" si="2"/>
-        <v>8005.4794520547957</v>
-      </c>
-      <c r="K28" s="9">
+        <v>5.0735667174023343E-2</v>
+      </c>
+      <c r="M28" s="9">
         <f t="shared" si="3"/>
-        <v>4090.8</v>
-      </c>
-      <c r="L28" s="10">
-        <f t="shared" si="0"/>
-        <v>5.0770417630991854E-2</v>
-      </c>
-      <c r="M28" s="11">
-        <f t="shared" si="1"/>
-        <v>1.2036755646817248</v>
+        <v>1.2044999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="8">
-        <v>805</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="B29" s="7">
+        <v>815</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="D29" s="5">
-        <f>D$37</f>
+        <f t="shared" ref="D29:E31" si="6">D$40</f>
         <v>0</v>
       </c>
       <c r="E29" s="5">
-        <f>E$37</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F29" s="6">
-        <f>F$37*$I29</f>
+        <f t="shared" ref="F29:F31" si="7">F$40*$I29</f>
         <v>0</v>
       </c>
       <c r="G29" s="6">
-        <f>G$37*$I29</f>
         <v>0</v>
       </c>
       <c r="H29" s="6">
-        <f>H$37*$I29</f>
-        <v>600</v>
-      </c>
-      <c r="I29" s="7">
-        <v>1500</v>
-      </c>
-      <c r="J29" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0</v>
+      </c>
+      <c r="J29" s="17">
+        <f t="shared" ref="J29" si="8">(D29*F29+E29*G29+(168-D29-E29)*H29)*365.25/7</f>
+        <v>4383</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" ref="K29" si="9">E29*G29*365.25/7</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="8" t="e">
+        <f t="shared" ref="L29" si="10">J29/365.25/24/I29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="9">
+        <f t="shared" ref="M29" si="11">MAX(F29,H29)/J29*365.25*24</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="7">
+        <v>825</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I30" s="16">
+        <v>0</v>
+      </c>
+      <c r="J30" s="17">
+        <f t="shared" si="0"/>
+        <v>4383</v>
+      </c>
+      <c r="K30" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="8" t="e">
         <f t="shared" si="2"/>
-        <v>5259600</v>
-      </c>
-      <c r="K29" s="9">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M30" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="10">
-        <f t="shared" si="0"/>
-        <v>0.40027397260273978</v>
-      </c>
-      <c r="M29" s="11">
-        <f t="shared" si="1"/>
-        <v>0.99931553730321698</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="B30" s="13"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="C31" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="A31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="7">
+        <v>835</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I31" s="16">
+        <v>0</v>
+      </c>
+      <c r="J31" s="17">
+        <f t="shared" ref="J31" si="12">(D31*F31+E31*G31+(168-D31-E31)*H31)*365.25/7</f>
+        <v>4383</v>
+      </c>
+      <c r="K31" s="17">
+        <f t="shared" ref="K31" si="13">E31*G31*365.25/7</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15" customHeight="1"/>
+    <row r="33" spans="1:9" ht="15" customHeight="1">
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" customHeight="1">
+      <c r="C34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1">
+      <c r="B35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1">
-      <c r="B32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="16">
+      <c r="D35" s="14">
         <v>35</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E35" s="14">
         <v>49</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F35" s="15">
         <v>0.8</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G35" s="15">
         <v>0.25</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H35" s="15">
         <v>0.38841324200913252</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15" customHeight="1">
-      <c r="B33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="16">
+      <c r="I35" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" customHeight="1">
+      <c r="B36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="14">
         <v>35</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E36" s="14">
         <v>49</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F36" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G36" s="15">
         <v>1.6</v>
       </c>
-      <c r="H33" s="17">
+      <c r="H36" s="15">
         <v>0.43481735159817364</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15" customHeight="1">
-      <c r="A34" s="1"/>
-      <c r="B34" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="16">
-        <v>66</v>
-      </c>
-      <c r="E34" s="16">
-        <v>0</v>
-      </c>
-      <c r="F34" s="17">
-        <v>0.7</v>
-      </c>
-      <c r="G34" s="17">
-        <v>0</v>
-      </c>
-      <c r="H34" s="17">
-        <v>0.20588235294117652</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1">
-      <c r="A35" s="1"/>
-      <c r="B35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="16">
-        <v>0</v>
-      </c>
-      <c r="E35" s="16">
-        <f>168/0.9*0.4</f>
-        <v>74.666666666666671</v>
-      </c>
-      <c r="F35" s="17">
-        <v>0</v>
-      </c>
-      <c r="G35" s="17">
-        <v>0.9</v>
-      </c>
-      <c r="H35" s="17">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15" customHeight="1">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="16">
-        <v>0</v>
-      </c>
-      <c r="E36" s="16">
-        <v>0</v>
-      </c>
-      <c r="F36" s="17">
-        <v>0</v>
-      </c>
-      <c r="G36" s="17">
-        <v>0</v>
-      </c>
-      <c r="H36" s="17">
-        <v>0.9</v>
-      </c>
       <c r="I36" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="16">
-        <v>0</v>
-      </c>
-      <c r="E37" s="16">
-        <v>0</v>
-      </c>
-      <c r="F37" s="17">
-        <v>0</v>
-      </c>
-      <c r="G37" s="17">
-        <v>0</v>
-      </c>
-      <c r="H37" s="17">
-        <v>0.4</v>
+        <v>28</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="14">
+        <v>66</v>
+      </c>
+      <c r="E37" s="14">
+        <v>0</v>
+      </c>
+      <c r="F37" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="G37" s="15">
+        <v>0</v>
+      </c>
+      <c r="H37" s="15">
+        <v>0.20588235294117652</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
+      <c r="B38" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="14">
+        <v>0</v>
+      </c>
+      <c r="E38" s="14">
+        <f>168/0.9*0.4</f>
+        <v>74.666666666666671</v>
+      </c>
+      <c r="F38" s="15">
+        <v>0</v>
+      </c>
+      <c r="G38" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H38" s="15">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" customHeight="1">
+      <c r="A39" s="1"/>
+      <c r="B39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="14">
+        <v>0</v>
+      </c>
+      <c r="E39" s="14">
+        <v>0</v>
+      </c>
+      <c r="F39" s="15">
+        <v>0</v>
+      </c>
+      <c r="G39" s="15">
+        <v>0</v>
+      </c>
+      <c r="H39" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" customHeight="1">
+      <c r="A40" s="1"/>
+      <c r="B40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="14">
+        <v>0</v>
+      </c>
+      <c r="E40" s="14">
+        <v>0</v>
+      </c>
+      <c r="F40" s="15">
+        <v>0</v>
+      </c>
+      <c r="G40" s="15">
+        <v>0</v>
+      </c>
+      <c r="H40" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" customHeight="1"/>
+    <row r="43" spans="1:9" ht="15" customHeight="1"/>
+    <row r="44" spans="1:9" ht="15" customHeight="1"/>
+    <row r="45" spans="1:9" ht="15" customHeight="1"/>
+    <row r="46" spans="1:9" ht="15" customHeight="1"/>
+    <row r="47" spans="1:9" ht="15" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A3:M29">
+  <autoFilter ref="A3:M30">
     <sortState ref="A4:M29">
       <sortCondition ref="B3:B29"/>
     </sortState>

</xml_diff>